<commit_message>
Created new page classes and new test classes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharmin Zaman\IdeaProjects\Dummy_Sites_Practice_Framework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Dummy_Sites_Practice_Framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CB2750-8D9C-47FB-9F9E-4FA8074ADE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B4AEFF-1440-4973-BC31-AD7B11E5BA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="940" windowWidth="14400" windowHeight="8760" activeTab="1" xr2:uid="{A7C16175-ABB4-4A61-8A9E-2317A65352C4}"/>
+    <workbookView xWindow="6300" yWindow="2835" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{A7C16175-ABB4-4A61-8A9E-2317A65352C4}"/>
   </bookViews>
   <sheets>
     <sheet name="RahulShettyCountries" sheetId="1" r:id="rId1"/>
     <sheet name="UITestingButton" sheetId="2" r:id="rId2"/>
+    <sheet name="OrangeHRMSearches" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>United</t>
   </si>
@@ -58,6 +59,15 @@
   </si>
   <si>
     <t>Nusrat</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Leave</t>
+  </si>
+  <si>
+    <t>Performance</t>
   </si>
 </sst>
 </file>
@@ -415,9 +425,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -425,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -433,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -441,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -456,36 +466,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A20A873-8029-4C2C-9317-09ADFD940010}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A92E523-1EF9-4705-AC6B-3F326393D663}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>